<commit_message>
Upload the local repository to the git hub
</commit_message>
<xml_diff>
--- a/Question List.xlsx
+++ b/Question List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Series</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,12 +153,23 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>FirefoxProfile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>about:config
+FirefoxProfile profile = new FireFoxprofile();
+profile.setPreference("","");
+capability.setCapability(FireFoxDriver.Profile,profile);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +192,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,9 +220,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -508,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -540,6 +561,14 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>